<commit_message>
resolved issue with while loopconditionals
</commit_message>
<xml_diff>
--- a/assets/excel/chip_counter.xlsx
+++ b/assets/excel/chip_counter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ktuten/Desktop/too_many_chips/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9533A11-35D2-FA48-98CA-AA70EEB341D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8820A995-B5C5-C246-8C39-CA98399CFD89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
     <t>Takis Pop (Fuego)</t>
   </si>
   <si>
-    <t>Ruffles (Cheddar &amp; Sour Cream)</t>
+    <t>Wavy Lays (Hickory BBQ)</t>
   </si>
 </sst>
 </file>
@@ -54,16 +54,8 @@
     <numFmt numFmtId="164" formatCode="mmm\-dd"/>
     <numFmt numFmtId="165" formatCode="hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -98,27 +90,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -134,21 +111,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -492,20 +466,19 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="1" max="3" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -513,10 +486,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>43419</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0.27083333333333331</v>
       </c>
       <c r="C2" t="s">
@@ -524,10 +497,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>43419</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.3576388888888889</v>
       </c>
       <c r="C3" t="s">
@@ -535,10 +508,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>43419</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0.4826388888888889</v>
       </c>
       <c r="C4" t="s">
@@ -546,10 +519,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>43419</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>0.6</v>
       </c>
       <c r="C5" t="s">
@@ -557,10 +530,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>43420</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>0.29236111111111113</v>
       </c>
       <c r="C6" t="s">
@@ -568,11 +541,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>43421</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.61149214782407402</v>
+      <c r="A7" s="2">
+        <v>43424</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.31013888888888891</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
shebang added for executable support
</commit_message>
<xml_diff>
--- a/assets/excel/chip_counter.xlsx
+++ b/assets/excel/chip_counter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ktuten/Desktop/too_many_chips/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8820A995-B5C5-C246-8C39-CA98399CFD89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A119CA2-0D4F-4F40-8C18-CC46BD049061}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>Chips</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t>Snack</t>
   </si>
   <si>
     <t>Date</t>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Wavy Lays (Hickory BBQ)</t>
+  </si>
+  <si>
+    <t>Pocky (Chocolate)</t>
   </si>
 </sst>
 </file>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -541,7 +544,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="4">
         <v>43424</v>
       </c>
       <c r="B7" s="3">
@@ -551,9 +554,21 @@
         <v>7</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>43424</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>